<commit_message>
table 3a 3b 4 binding
</commit_message>
<xml_diff>
--- a/uds2018info_T5_T5A.xlsx
+++ b/uds2018info_T5_T5A.xlsx
@@ -566,7 +566,7 @@
     <t xml:space="preserve">Access Health Louisiana</t>
   </si>
   <si>
-    <t xml:space="preserve">843 Milling Ave</t>
+    <t xml:space="preserve">843 MILLING AVE</t>
   </si>
   <si>
     <t xml:space="preserve">Luling</t>
@@ -653,7 +653,7 @@
     <t xml:space="preserve">Baton Rouge Primary Care Collaborative, Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">220 Saint Vincent De Paul Dr</t>
+    <t xml:space="preserve">220 SAINT VINCENT DE PAUL DR</t>
   </si>
   <si>
     <t xml:space="preserve">Baton Rouge</t>
@@ -707,7 +707,7 @@
     <t xml:space="preserve">C A S S E Dental Health Institute</t>
   </si>
   <si>
-    <t xml:space="preserve">2120 Bert Kouns Industrial Loop Ste A</t>
+    <t xml:space="preserve">2120 BERT KOUNS INDUSTRIAL LOOP STE A</t>
   </si>
   <si>
     <t xml:space="preserve">Mansfield</t>
@@ -839,7 +839,7 @@
     <t xml:space="preserve">Catahoula Parish Hospital District # 2</t>
   </si>
   <si>
-    <t xml:space="preserve">307 Chisum St</t>
+    <t xml:space="preserve">307 chisum st</t>
   </si>
   <si>
     <t xml:space="preserve">SICILY ISLAND</t>
@@ -998,7 +998,7 @@
     <t xml:space="preserve">Excelth Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">1515 Poydras St Ste 1070</t>
+    <t xml:space="preserve">1515 POYDRAS ST STE 1070</t>
   </si>
   <si>
     <t xml:space="preserve">70112</t>
@@ -1085,7 +1085,7 @@
     <t xml:space="preserve">Hospital Service District No. 1-A Of The Parish Of Richland</t>
   </si>
   <si>
-    <t xml:space="preserve">407 Cincinnati St</t>
+    <t xml:space="preserve">407 CINCINNATI ST</t>
   </si>
   <si>
     <t xml:space="preserve">Delhi</t>
@@ -1139,7 +1139,7 @@
     <t xml:space="preserve">Iberia Comprehensive Community Health Center</t>
   </si>
   <si>
-    <t xml:space="preserve">806 Jefferson Terrace</t>
+    <t xml:space="preserve">806 JEFFERSON TERRACE</t>
   </si>
   <si>
     <t xml:space="preserve">New Iberia</t>
@@ -1199,7 +1199,7 @@
     <t xml:space="preserve">Innis Community Health Center, Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">6450 La Highway 1</t>
+    <t xml:space="preserve">6450 LA HIGHWAY 1</t>
   </si>
   <si>
     <t xml:space="preserve">Innis</t>
@@ -1253,7 +1253,7 @@
     <t xml:space="preserve">Jefferson Community Health Care Centers, Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">4028 Us Hwy 90 W</t>
+    <t xml:space="preserve">4028 US Hwy 90 W</t>
   </si>
   <si>
     <t xml:space="preserve">Avondale</t>
@@ -1316,7 +1316,7 @@
     <t xml:space="preserve">Jefferson Parish Human Services Authority</t>
   </si>
   <si>
-    <t xml:space="preserve">3616 S I 10 Service Rd W</t>
+    <t xml:space="preserve">3616 S I 10 SERVICE RD W</t>
   </si>
   <si>
     <t xml:space="preserve">Metairie</t>
@@ -1373,7 +1373,7 @@
     <t xml:space="preserve">Marillac Community Health Centers</t>
   </si>
   <si>
-    <t xml:space="preserve">3201 S Carrollton Ave</t>
+    <t xml:space="preserve">3201 S CARROLLTON AVE</t>
   </si>
   <si>
     <t xml:space="preserve">70118</t>
@@ -1436,7 +1436,7 @@
     <t xml:space="preserve">Morehouse Community Medical Centers, Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">518 Durham St</t>
+    <t xml:space="preserve">518 DURHAM ST</t>
   </si>
   <si>
     <t xml:space="preserve">Bastrop</t>
@@ -1595,7 +1595,7 @@
     <t xml:space="preserve">New Orleans Health Department</t>
   </si>
   <si>
-    <t xml:space="preserve">1300 Perdido St Bsmt</t>
+    <t xml:space="preserve">1300 PERDIDO ST BSMT</t>
   </si>
   <si>
     <t xml:space="preserve">Ragan  Collins</t>
@@ -1634,7 +1634,7 @@
     <t xml:space="preserve">Odyssey House Louisiana, Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">1125 N Tonti St</t>
+    <t xml:space="preserve">1125 N TONTI ST</t>
   </si>
   <si>
     <t xml:space="preserve">70119</t>
@@ -1817,7 +1817,7 @@
     <t xml:space="preserve">Primary Health Services Center</t>
   </si>
   <si>
-    <t xml:space="preserve">2914 Betin Ave</t>
+    <t xml:space="preserve">2914 BETIN AVE</t>
   </si>
   <si>
     <t xml:space="preserve">Monroe</t>
@@ -1868,7 +1868,7 @@
     <t xml:space="preserve">Priority Health Care</t>
   </si>
   <si>
-    <t xml:space="preserve">4700 Wichers Dr Ste 300</t>
+    <t xml:space="preserve">4700 WICHERS DR STE 300</t>
   </si>
   <si>
     <t xml:space="preserve">Marrero</t>
@@ -2027,7 +2027,7 @@
     <t xml:space="preserve">Southwest Louisiana Primary Health Care Ctr, Inc.</t>
   </si>
   <si>
-    <t xml:space="preserve">8762 Hwy 182</t>
+    <t xml:space="preserve">8762 HWY 182</t>
   </si>
   <si>
     <t xml:space="preserve">Opelousas</t>
@@ -2186,7 +2186,7 @@
     <t xml:space="preserve">Start Corporation</t>
   </si>
   <si>
-    <t xml:space="preserve">420 Magnolia St</t>
+    <t xml:space="preserve">420 MAGNOLIA ST</t>
   </si>
   <si>
     <t xml:space="preserve">Houma</t>
@@ -2420,7 +2420,7 @@
     <t xml:space="preserve">Winn Community Health Center, Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">201 Cherokee Dr</t>
+    <t xml:space="preserve">201 CHEROKEE DR</t>
   </si>
   <si>
     <t xml:space="preserve">Winnfield</t>
@@ -19008,1100 +19008,6 @@
       <c r="FW35"/>
       <c r="FX35"/>
     </row>
-    <row r="36">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36"/>
-      <c r="AG36"/>
-      <c r="AH36"/>
-      <c r="AI36"/>
-      <c r="AJ36"/>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36"/>
-      <c r="AN36"/>
-      <c r="AO36"/>
-      <c r="AP36"/>
-      <c r="AQ36"/>
-      <c r="AR36"/>
-      <c r="AS36"/>
-      <c r="AT36"/>
-      <c r="AU36"/>
-      <c r="AV36"/>
-      <c r="AW36"/>
-      <c r="AX36"/>
-      <c r="AY36"/>
-      <c r="AZ36"/>
-      <c r="BA36"/>
-      <c r="BB36"/>
-      <c r="BC36"/>
-      <c r="BD36"/>
-      <c r="BE36"/>
-      <c r="BF36"/>
-      <c r="BG36"/>
-      <c r="BH36"/>
-      <c r="BI36"/>
-      <c r="BJ36"/>
-      <c r="BK36"/>
-      <c r="BL36"/>
-      <c r="BM36"/>
-      <c r="BN36"/>
-      <c r="BO36"/>
-      <c r="BP36"/>
-      <c r="BQ36"/>
-      <c r="BR36"/>
-      <c r="BS36"/>
-      <c r="BT36"/>
-      <c r="BU36"/>
-      <c r="BV36"/>
-      <c r="BW36"/>
-      <c r="BX36"/>
-      <c r="BY36"/>
-      <c r="BZ36"/>
-      <c r="CA36"/>
-      <c r="CB36"/>
-      <c r="CC36"/>
-      <c r="CD36"/>
-      <c r="CE36"/>
-      <c r="CF36"/>
-      <c r="CG36"/>
-      <c r="CH36"/>
-      <c r="CI36"/>
-      <c r="CJ36"/>
-      <c r="CK36"/>
-      <c r="CL36"/>
-      <c r="CM36"/>
-      <c r="CN36"/>
-      <c r="CO36"/>
-      <c r="CP36"/>
-      <c r="CQ36"/>
-      <c r="CR36"/>
-      <c r="CS36"/>
-      <c r="CT36"/>
-      <c r="CU36"/>
-      <c r="CV36"/>
-      <c r="CW36"/>
-      <c r="CX36"/>
-      <c r="CY36"/>
-      <c r="CZ36"/>
-      <c r="DA36"/>
-      <c r="DB36"/>
-      <c r="DC36"/>
-      <c r="DD36"/>
-      <c r="DE36"/>
-      <c r="DF36"/>
-      <c r="DG36"/>
-      <c r="DH36"/>
-      <c r="DI36"/>
-      <c r="DJ36"/>
-      <c r="DK36"/>
-      <c r="DL36"/>
-      <c r="DM36"/>
-      <c r="DN36"/>
-      <c r="DO36"/>
-      <c r="DP36"/>
-      <c r="DQ36"/>
-      <c r="DR36"/>
-      <c r="DS36"/>
-      <c r="DT36"/>
-      <c r="DU36"/>
-      <c r="DV36"/>
-      <c r="DW36"/>
-      <c r="DX36"/>
-      <c r="DY36"/>
-      <c r="DZ36"/>
-      <c r="EA36"/>
-      <c r="EB36"/>
-      <c r="EC36"/>
-      <c r="ED36"/>
-      <c r="EE36"/>
-      <c r="EF36"/>
-      <c r="EG36"/>
-      <c r="EH36"/>
-      <c r="EI36"/>
-      <c r="EJ36"/>
-      <c r="EK36"/>
-      <c r="EL36"/>
-      <c r="EM36"/>
-      <c r="EN36"/>
-      <c r="EO36"/>
-      <c r="EP36"/>
-      <c r="EQ36"/>
-      <c r="ER36"/>
-      <c r="ES36"/>
-      <c r="ET36"/>
-      <c r="EU36"/>
-      <c r="EV36"/>
-      <c r="EW36"/>
-      <c r="EX36"/>
-      <c r="EY36"/>
-      <c r="EZ36"/>
-      <c r="FA36"/>
-      <c r="FB36"/>
-      <c r="FC36"/>
-      <c r="FD36"/>
-      <c r="FE36"/>
-      <c r="FF36"/>
-      <c r="FG36"/>
-      <c r="FH36"/>
-      <c r="FI36"/>
-      <c r="FJ36"/>
-      <c r="FK36"/>
-      <c r="FL36"/>
-      <c r="FM36"/>
-      <c r="FN36"/>
-      <c r="FO36"/>
-      <c r="FP36"/>
-      <c r="FQ36"/>
-      <c r="FR36"/>
-      <c r="FS36"/>
-      <c r="FT36"/>
-      <c r="FU36"/>
-      <c r="FV36"/>
-      <c r="FW36"/>
-      <c r="FX36"/>
-    </row>
-    <row r="37">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-      <c r="O37"/>
-      <c r="P37"/>
-      <c r="Q37"/>
-      <c r="R37"/>
-      <c r="S37"/>
-      <c r="T37"/>
-      <c r="U37"/>
-      <c r="V37"/>
-      <c r="W37"/>
-      <c r="X37"/>
-      <c r="Y37"/>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37"/>
-      <c r="AD37"/>
-      <c r="AE37"/>
-      <c r="AF37"/>
-      <c r="AG37"/>
-      <c r="AH37"/>
-      <c r="AI37"/>
-      <c r="AJ37"/>
-      <c r="AK37"/>
-      <c r="AL37"/>
-      <c r="AM37"/>
-      <c r="AN37"/>
-      <c r="AO37"/>
-      <c r="AP37"/>
-      <c r="AQ37"/>
-      <c r="AR37"/>
-      <c r="AS37"/>
-      <c r="AT37"/>
-      <c r="AU37"/>
-      <c r="AV37"/>
-      <c r="AW37"/>
-      <c r="AX37"/>
-      <c r="AY37"/>
-      <c r="AZ37"/>
-      <c r="BA37"/>
-      <c r="BB37"/>
-      <c r="BC37"/>
-      <c r="BD37"/>
-      <c r="BE37"/>
-      <c r="BF37"/>
-      <c r="BG37"/>
-      <c r="BH37"/>
-      <c r="BI37"/>
-      <c r="BJ37"/>
-      <c r="BK37"/>
-      <c r="BL37"/>
-      <c r="BM37"/>
-      <c r="BN37"/>
-      <c r="BO37"/>
-      <c r="BP37"/>
-      <c r="BQ37"/>
-      <c r="BR37"/>
-      <c r="BS37"/>
-      <c r="BT37"/>
-      <c r="BU37"/>
-      <c r="BV37"/>
-      <c r="BW37"/>
-      <c r="BX37"/>
-      <c r="BY37"/>
-      <c r="BZ37"/>
-      <c r="CA37"/>
-      <c r="CB37"/>
-      <c r="CC37"/>
-      <c r="CD37"/>
-      <c r="CE37"/>
-      <c r="CF37"/>
-      <c r="CG37"/>
-      <c r="CH37"/>
-      <c r="CI37"/>
-      <c r="CJ37"/>
-      <c r="CK37"/>
-      <c r="CL37"/>
-      <c r="CM37"/>
-      <c r="CN37"/>
-      <c r="CO37"/>
-      <c r="CP37"/>
-      <c r="CQ37"/>
-      <c r="CR37"/>
-      <c r="CS37"/>
-      <c r="CT37"/>
-      <c r="CU37"/>
-      <c r="CV37"/>
-      <c r="CW37"/>
-      <c r="CX37"/>
-      <c r="CY37"/>
-      <c r="CZ37"/>
-      <c r="DA37"/>
-      <c r="DB37"/>
-      <c r="DC37"/>
-      <c r="DD37"/>
-      <c r="DE37"/>
-      <c r="DF37"/>
-      <c r="DG37"/>
-      <c r="DH37"/>
-      <c r="DI37"/>
-      <c r="DJ37"/>
-      <c r="DK37"/>
-      <c r="DL37"/>
-      <c r="DM37"/>
-      <c r="DN37"/>
-      <c r="DO37"/>
-      <c r="DP37"/>
-      <c r="DQ37"/>
-      <c r="DR37"/>
-      <c r="DS37"/>
-      <c r="DT37"/>
-      <c r="DU37"/>
-      <c r="DV37"/>
-      <c r="DW37"/>
-      <c r="DX37"/>
-      <c r="DY37"/>
-      <c r="DZ37"/>
-      <c r="EA37"/>
-      <c r="EB37"/>
-      <c r="EC37"/>
-      <c r="ED37"/>
-      <c r="EE37"/>
-      <c r="EF37"/>
-      <c r="EG37"/>
-      <c r="EH37"/>
-      <c r="EI37"/>
-      <c r="EJ37"/>
-      <c r="EK37"/>
-      <c r="EL37"/>
-      <c r="EM37"/>
-      <c r="EN37"/>
-      <c r="EO37"/>
-      <c r="EP37"/>
-      <c r="EQ37"/>
-      <c r="ER37"/>
-      <c r="ES37"/>
-      <c r="ET37"/>
-      <c r="EU37"/>
-      <c r="EV37"/>
-      <c r="EW37"/>
-      <c r="EX37"/>
-      <c r="EY37"/>
-      <c r="EZ37"/>
-      <c r="FA37"/>
-      <c r="FB37"/>
-      <c r="FC37"/>
-      <c r="FD37"/>
-      <c r="FE37"/>
-      <c r="FF37"/>
-      <c r="FG37"/>
-      <c r="FH37"/>
-      <c r="FI37"/>
-      <c r="FJ37"/>
-      <c r="FK37"/>
-      <c r="FL37"/>
-      <c r="FM37"/>
-      <c r="FN37"/>
-      <c r="FO37"/>
-      <c r="FP37"/>
-      <c r="FQ37"/>
-      <c r="FR37"/>
-      <c r="FS37"/>
-      <c r="FT37"/>
-      <c r="FU37"/>
-      <c r="FV37"/>
-      <c r="FW37"/>
-      <c r="FX37"/>
-    </row>
-    <row r="38">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-      <c r="N38"/>
-      <c r="O38"/>
-      <c r="P38"/>
-      <c r="Q38"/>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
-      <c r="W38"/>
-      <c r="X38"/>
-      <c r="Y38"/>
-      <c r="Z38"/>
-      <c r="AA38"/>
-      <c r="AB38"/>
-      <c r="AC38"/>
-      <c r="AD38"/>
-      <c r="AE38"/>
-      <c r="AF38"/>
-      <c r="AG38"/>
-      <c r="AH38"/>
-      <c r="AI38"/>
-      <c r="AJ38"/>
-      <c r="AK38"/>
-      <c r="AL38"/>
-      <c r="AM38"/>
-      <c r="AN38"/>
-      <c r="AO38"/>
-      <c r="AP38"/>
-      <c r="AQ38"/>
-      <c r="AR38"/>
-      <c r="AS38"/>
-      <c r="AT38"/>
-      <c r="AU38"/>
-      <c r="AV38"/>
-      <c r="AW38"/>
-      <c r="AX38"/>
-      <c r="AY38"/>
-      <c r="AZ38"/>
-      <c r="BA38"/>
-      <c r="BB38"/>
-      <c r="BC38"/>
-      <c r="BD38"/>
-      <c r="BE38"/>
-      <c r="BF38"/>
-      <c r="BG38"/>
-      <c r="BH38"/>
-      <c r="BI38"/>
-      <c r="BJ38"/>
-      <c r="BK38"/>
-      <c r="BL38"/>
-      <c r="BM38"/>
-      <c r="BN38"/>
-      <c r="BO38"/>
-      <c r="BP38"/>
-      <c r="BQ38"/>
-      <c r="BR38"/>
-      <c r="BS38"/>
-      <c r="BT38"/>
-      <c r="BU38"/>
-      <c r="BV38"/>
-      <c r="BW38"/>
-      <c r="BX38"/>
-      <c r="BY38"/>
-      <c r="BZ38"/>
-      <c r="CA38"/>
-      <c r="CB38"/>
-      <c r="CC38"/>
-      <c r="CD38"/>
-      <c r="CE38"/>
-      <c r="CF38"/>
-      <c r="CG38"/>
-      <c r="CH38"/>
-      <c r="CI38"/>
-      <c r="CJ38"/>
-      <c r="CK38"/>
-      <c r="CL38"/>
-      <c r="CM38"/>
-      <c r="CN38"/>
-      <c r="CO38"/>
-      <c r="CP38"/>
-      <c r="CQ38"/>
-      <c r="CR38"/>
-      <c r="CS38"/>
-      <c r="CT38"/>
-      <c r="CU38"/>
-      <c r="CV38"/>
-      <c r="CW38"/>
-      <c r="CX38"/>
-      <c r="CY38"/>
-      <c r="CZ38"/>
-      <c r="DA38"/>
-      <c r="DB38"/>
-      <c r="DC38"/>
-      <c r="DD38"/>
-      <c r="DE38"/>
-      <c r="DF38"/>
-      <c r="DG38"/>
-      <c r="DH38"/>
-      <c r="DI38"/>
-      <c r="DJ38"/>
-      <c r="DK38"/>
-      <c r="DL38"/>
-      <c r="DM38"/>
-      <c r="DN38"/>
-      <c r="DO38"/>
-      <c r="DP38"/>
-      <c r="DQ38"/>
-      <c r="DR38"/>
-      <c r="DS38"/>
-      <c r="DT38"/>
-      <c r="DU38"/>
-      <c r="DV38"/>
-      <c r="DW38"/>
-      <c r="DX38"/>
-      <c r="DY38"/>
-      <c r="DZ38"/>
-      <c r="EA38"/>
-      <c r="EB38"/>
-      <c r="EC38"/>
-      <c r="ED38"/>
-      <c r="EE38"/>
-      <c r="EF38"/>
-      <c r="EG38"/>
-      <c r="EH38"/>
-      <c r="EI38"/>
-      <c r="EJ38"/>
-      <c r="EK38"/>
-      <c r="EL38"/>
-      <c r="EM38"/>
-      <c r="EN38"/>
-      <c r="EO38"/>
-      <c r="EP38"/>
-      <c r="EQ38"/>
-      <c r="ER38"/>
-      <c r="ES38"/>
-      <c r="ET38"/>
-      <c r="EU38"/>
-      <c r="EV38"/>
-      <c r="EW38"/>
-      <c r="EX38"/>
-      <c r="EY38"/>
-      <c r="EZ38"/>
-      <c r="FA38"/>
-      <c r="FB38"/>
-      <c r="FC38"/>
-      <c r="FD38"/>
-      <c r="FE38"/>
-      <c r="FF38"/>
-      <c r="FG38"/>
-      <c r="FH38"/>
-      <c r="FI38"/>
-      <c r="FJ38"/>
-      <c r="FK38"/>
-      <c r="FL38"/>
-      <c r="FM38"/>
-      <c r="FN38"/>
-      <c r="FO38"/>
-      <c r="FP38"/>
-      <c r="FQ38"/>
-      <c r="FR38"/>
-      <c r="FS38"/>
-      <c r="FT38"/>
-      <c r="FU38"/>
-      <c r="FV38"/>
-      <c r="FW38"/>
-      <c r="FX38"/>
-    </row>
-    <row r="39">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
-      <c r="AE39"/>
-      <c r="AF39"/>
-      <c r="AG39"/>
-      <c r="AH39"/>
-      <c r="AI39"/>
-      <c r="AJ39"/>
-      <c r="AK39"/>
-      <c r="AL39"/>
-      <c r="AM39"/>
-      <c r="AN39"/>
-      <c r="AO39"/>
-      <c r="AP39"/>
-      <c r="AQ39"/>
-      <c r="AR39"/>
-      <c r="AS39"/>
-      <c r="AT39"/>
-      <c r="AU39"/>
-      <c r="AV39"/>
-      <c r="AW39"/>
-      <c r="AX39"/>
-      <c r="AY39"/>
-      <c r="AZ39"/>
-      <c r="BA39"/>
-      <c r="BB39"/>
-      <c r="BC39"/>
-      <c r="BD39"/>
-      <c r="BE39"/>
-      <c r="BF39"/>
-      <c r="BG39"/>
-      <c r="BH39"/>
-      <c r="BI39"/>
-      <c r="BJ39"/>
-      <c r="BK39"/>
-      <c r="BL39"/>
-      <c r="BM39"/>
-      <c r="BN39"/>
-      <c r="BO39"/>
-      <c r="BP39"/>
-      <c r="BQ39"/>
-      <c r="BR39"/>
-      <c r="BS39"/>
-      <c r="BT39"/>
-      <c r="BU39"/>
-      <c r="BV39"/>
-      <c r="BW39"/>
-      <c r="BX39"/>
-      <c r="BY39"/>
-      <c r="BZ39"/>
-      <c r="CA39"/>
-      <c r="CB39"/>
-      <c r="CC39"/>
-      <c r="CD39"/>
-      <c r="CE39"/>
-      <c r="CF39"/>
-      <c r="CG39"/>
-      <c r="CH39"/>
-      <c r="CI39"/>
-      <c r="CJ39"/>
-      <c r="CK39"/>
-      <c r="CL39"/>
-      <c r="CM39"/>
-      <c r="CN39"/>
-      <c r="CO39"/>
-      <c r="CP39"/>
-      <c r="CQ39"/>
-      <c r="CR39"/>
-      <c r="CS39"/>
-      <c r="CT39"/>
-      <c r="CU39"/>
-      <c r="CV39"/>
-      <c r="CW39"/>
-      <c r="CX39"/>
-      <c r="CY39"/>
-      <c r="CZ39"/>
-      <c r="DA39"/>
-      <c r="DB39"/>
-      <c r="DC39"/>
-      <c r="DD39"/>
-      <c r="DE39"/>
-      <c r="DF39"/>
-      <c r="DG39"/>
-      <c r="DH39"/>
-      <c r="DI39"/>
-      <c r="DJ39"/>
-      <c r="DK39"/>
-      <c r="DL39"/>
-      <c r="DM39"/>
-      <c r="DN39"/>
-      <c r="DO39"/>
-      <c r="DP39"/>
-      <c r="DQ39"/>
-      <c r="DR39"/>
-      <c r="DS39"/>
-      <c r="DT39"/>
-      <c r="DU39"/>
-      <c r="DV39"/>
-      <c r="DW39"/>
-      <c r="DX39"/>
-      <c r="DY39"/>
-      <c r="DZ39"/>
-      <c r="EA39"/>
-      <c r="EB39"/>
-      <c r="EC39"/>
-      <c r="ED39"/>
-      <c r="EE39"/>
-      <c r="EF39"/>
-      <c r="EG39"/>
-      <c r="EH39"/>
-      <c r="EI39"/>
-      <c r="EJ39"/>
-      <c r="EK39"/>
-      <c r="EL39"/>
-      <c r="EM39"/>
-      <c r="EN39"/>
-      <c r="EO39"/>
-      <c r="EP39"/>
-      <c r="EQ39"/>
-      <c r="ER39"/>
-      <c r="ES39"/>
-      <c r="ET39"/>
-      <c r="EU39"/>
-      <c r="EV39"/>
-      <c r="EW39"/>
-      <c r="EX39"/>
-      <c r="EY39"/>
-      <c r="EZ39"/>
-      <c r="FA39"/>
-      <c r="FB39"/>
-      <c r="FC39"/>
-      <c r="FD39"/>
-      <c r="FE39"/>
-      <c r="FF39"/>
-      <c r="FG39"/>
-      <c r="FH39"/>
-      <c r="FI39"/>
-      <c r="FJ39"/>
-      <c r="FK39"/>
-      <c r="FL39"/>
-      <c r="FM39"/>
-      <c r="FN39"/>
-      <c r="FO39"/>
-      <c r="FP39"/>
-      <c r="FQ39"/>
-      <c r="FR39"/>
-      <c r="FS39"/>
-      <c r="FT39"/>
-      <c r="FU39"/>
-      <c r="FV39"/>
-      <c r="FW39"/>
-      <c r="FX39"/>
-    </row>
-    <row r="40">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
-      <c r="AE40"/>
-      <c r="AF40"/>
-      <c r="AG40"/>
-      <c r="AH40"/>
-      <c r="AI40"/>
-      <c r="AJ40"/>
-      <c r="AK40"/>
-      <c r="AL40"/>
-      <c r="AM40"/>
-      <c r="AN40"/>
-      <c r="AO40"/>
-      <c r="AP40"/>
-      <c r="AQ40"/>
-      <c r="AR40"/>
-      <c r="AS40"/>
-      <c r="AT40"/>
-      <c r="AU40"/>
-      <c r="AV40"/>
-      <c r="AW40"/>
-      <c r="AX40"/>
-      <c r="AY40"/>
-      <c r="AZ40"/>
-      <c r="BA40"/>
-      <c r="BB40"/>
-      <c r="BC40"/>
-      <c r="BD40"/>
-      <c r="BE40"/>
-      <c r="BF40"/>
-      <c r="BG40"/>
-      <c r="BH40"/>
-      <c r="BI40"/>
-      <c r="BJ40"/>
-      <c r="BK40"/>
-      <c r="BL40"/>
-      <c r="BM40"/>
-      <c r="BN40"/>
-      <c r="BO40"/>
-      <c r="BP40"/>
-      <c r="BQ40"/>
-      <c r="BR40"/>
-      <c r="BS40"/>
-      <c r="BT40"/>
-      <c r="BU40"/>
-      <c r="BV40"/>
-      <c r="BW40"/>
-      <c r="BX40"/>
-      <c r="BY40"/>
-      <c r="BZ40"/>
-      <c r="CA40"/>
-      <c r="CB40"/>
-      <c r="CC40"/>
-      <c r="CD40"/>
-      <c r="CE40"/>
-      <c r="CF40"/>
-      <c r="CG40"/>
-      <c r="CH40"/>
-      <c r="CI40"/>
-      <c r="CJ40"/>
-      <c r="CK40"/>
-      <c r="CL40"/>
-      <c r="CM40"/>
-      <c r="CN40"/>
-      <c r="CO40"/>
-      <c r="CP40"/>
-      <c r="CQ40"/>
-      <c r="CR40"/>
-      <c r="CS40"/>
-      <c r="CT40"/>
-      <c r="CU40"/>
-      <c r="CV40"/>
-      <c r="CW40"/>
-      <c r="CX40"/>
-      <c r="CY40"/>
-      <c r="CZ40"/>
-      <c r="DA40"/>
-      <c r="DB40"/>
-      <c r="DC40"/>
-      <c r="DD40"/>
-      <c r="DE40"/>
-      <c r="DF40"/>
-      <c r="DG40"/>
-      <c r="DH40"/>
-      <c r="DI40"/>
-      <c r="DJ40"/>
-      <c r="DK40"/>
-      <c r="DL40"/>
-      <c r="DM40"/>
-      <c r="DN40"/>
-      <c r="DO40"/>
-      <c r="DP40"/>
-      <c r="DQ40"/>
-      <c r="DR40"/>
-      <c r="DS40"/>
-      <c r="DT40"/>
-      <c r="DU40"/>
-      <c r="DV40"/>
-      <c r="DW40"/>
-      <c r="DX40"/>
-      <c r="DY40"/>
-      <c r="DZ40"/>
-      <c r="EA40"/>
-      <c r="EB40"/>
-      <c r="EC40"/>
-      <c r="ED40"/>
-      <c r="EE40"/>
-      <c r="EF40"/>
-      <c r="EG40"/>
-      <c r="EH40"/>
-      <c r="EI40"/>
-      <c r="EJ40"/>
-      <c r="EK40"/>
-      <c r="EL40"/>
-      <c r="EM40"/>
-      <c r="EN40"/>
-      <c r="EO40"/>
-      <c r="EP40"/>
-      <c r="EQ40"/>
-      <c r="ER40"/>
-      <c r="ES40"/>
-      <c r="ET40"/>
-      <c r="EU40"/>
-      <c r="EV40"/>
-      <c r="EW40"/>
-      <c r="EX40"/>
-      <c r="EY40"/>
-      <c r="EZ40"/>
-      <c r="FA40"/>
-      <c r="FB40"/>
-      <c r="FC40"/>
-      <c r="FD40"/>
-      <c r="FE40"/>
-      <c r="FF40"/>
-      <c r="FG40"/>
-      <c r="FH40"/>
-      <c r="FI40"/>
-      <c r="FJ40"/>
-      <c r="FK40"/>
-      <c r="FL40"/>
-      <c r="FM40"/>
-      <c r="FN40"/>
-      <c r="FO40"/>
-      <c r="FP40"/>
-      <c r="FQ40"/>
-      <c r="FR40"/>
-      <c r="FS40"/>
-      <c r="FT40"/>
-      <c r="FU40"/>
-      <c r="FV40"/>
-      <c r="FW40"/>
-      <c r="FX40"/>
-    </row>
-    <row r="41">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-      <c r="O41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-      <c r="R41"/>
-      <c r="S41"/>
-      <c r="T41"/>
-      <c r="U41"/>
-      <c r="V41"/>
-      <c r="W41"/>
-      <c r="X41"/>
-      <c r="Y41"/>
-      <c r="Z41"/>
-      <c r="AA41"/>
-      <c r="AB41"/>
-      <c r="AC41"/>
-      <c r="AD41"/>
-      <c r="AE41"/>
-      <c r="AF41"/>
-      <c r="AG41"/>
-      <c r="AH41"/>
-      <c r="AI41"/>
-      <c r="AJ41"/>
-      <c r="AK41"/>
-      <c r="AL41"/>
-      <c r="AM41"/>
-      <c r="AN41"/>
-      <c r="AO41"/>
-      <c r="AP41"/>
-      <c r="AQ41"/>
-      <c r="AR41"/>
-      <c r="AS41"/>
-      <c r="AT41"/>
-      <c r="AU41"/>
-      <c r="AV41"/>
-      <c r="AW41"/>
-      <c r="AX41"/>
-      <c r="AY41"/>
-      <c r="AZ41"/>
-      <c r="BA41"/>
-      <c r="BB41"/>
-      <c r="BC41"/>
-      <c r="BD41"/>
-      <c r="BE41"/>
-      <c r="BF41"/>
-      <c r="BG41"/>
-      <c r="BH41"/>
-      <c r="BI41" t="n">
-        <v>16.59</v>
-      </c>
-      <c r="BJ41"/>
-      <c r="BK41"/>
-      <c r="BL41"/>
-      <c r="BM41"/>
-      <c r="BN41"/>
-      <c r="BO41"/>
-      <c r="BP41"/>
-      <c r="BQ41"/>
-      <c r="BR41"/>
-      <c r="BS41"/>
-      <c r="BT41"/>
-      <c r="BU41"/>
-      <c r="BV41"/>
-      <c r="BW41"/>
-      <c r="BX41"/>
-      <c r="BY41"/>
-      <c r="BZ41"/>
-      <c r="CA41"/>
-      <c r="CB41"/>
-      <c r="CC41"/>
-      <c r="CD41"/>
-      <c r="CE41"/>
-      <c r="CF41"/>
-      <c r="CG41"/>
-      <c r="CH41"/>
-      <c r="CI41"/>
-      <c r="CJ41"/>
-      <c r="CK41"/>
-      <c r="CL41"/>
-      <c r="CM41"/>
-      <c r="CN41"/>
-      <c r="CO41"/>
-      <c r="CP41"/>
-      <c r="CQ41"/>
-      <c r="CR41"/>
-      <c r="CS41"/>
-      <c r="CT41"/>
-      <c r="CU41"/>
-      <c r="CV41"/>
-      <c r="CW41"/>
-      <c r="CX41"/>
-      <c r="CY41"/>
-      <c r="CZ41"/>
-      <c r="DA41"/>
-      <c r="DB41"/>
-      <c r="DC41"/>
-      <c r="DD41"/>
-      <c r="DE41"/>
-      <c r="DF41"/>
-      <c r="DG41"/>
-      <c r="DH41"/>
-      <c r="DI41"/>
-      <c r="DJ41"/>
-      <c r="DK41"/>
-      <c r="DL41"/>
-      <c r="DM41"/>
-      <c r="DN41"/>
-      <c r="DO41"/>
-      <c r="DP41"/>
-      <c r="DQ41"/>
-      <c r="DR41"/>
-      <c r="DS41"/>
-      <c r="DT41"/>
-      <c r="DU41"/>
-      <c r="DV41"/>
-      <c r="DW41"/>
-      <c r="DX41"/>
-      <c r="DY41"/>
-      <c r="DZ41"/>
-      <c r="EA41"/>
-      <c r="EB41"/>
-      <c r="EC41"/>
-      <c r="ED41"/>
-      <c r="EE41"/>
-      <c r="EF41"/>
-      <c r="EG41"/>
-      <c r="EH41"/>
-      <c r="EI41"/>
-      <c r="EJ41"/>
-      <c r="EK41"/>
-      <c r="EL41"/>
-      <c r="EM41"/>
-      <c r="EN41"/>
-      <c r="EO41"/>
-      <c r="EP41"/>
-      <c r="EQ41"/>
-      <c r="ER41"/>
-      <c r="ES41"/>
-      <c r="ET41"/>
-      <c r="EU41"/>
-      <c r="EV41"/>
-      <c r="EW41"/>
-      <c r="EX41"/>
-      <c r="EY41"/>
-      <c r="EZ41"/>
-      <c r="FA41"/>
-      <c r="FB41"/>
-      <c r="FC41"/>
-      <c r="FD41"/>
-      <c r="FE41"/>
-      <c r="FF41"/>
-      <c r="FG41"/>
-      <c r="FH41"/>
-      <c r="FI41"/>
-      <c r="FJ41"/>
-      <c r="FK41"/>
-      <c r="FL41"/>
-      <c r="FM41"/>
-      <c r="FN41"/>
-      <c r="FO41"/>
-      <c r="FP41"/>
-      <c r="FQ41"/>
-      <c r="FR41"/>
-      <c r="FS41"/>
-      <c r="FT41"/>
-      <c r="FU41"/>
-      <c r="FV41"/>
-      <c r="FW41"/>
-      <c r="FX41"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>